<commit_message>
Fix : Data peserta
</commit_message>
<xml_diff>
--- a/storage/datauser/datapeserta.xlsx
+++ b/storage/datauser/datapeserta.xlsx
@@ -3087,8 +3087,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="B111" sqref="B111"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3168,10 +3168,10 @@
       </c>
       <c r="C2">
         <f ca="1">INT(RAND()*(99999999-10000000+1)+10000000)</f>
-        <v>99500984</v>
+        <v>16436724</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E2">
         <v>3</v>
@@ -3199,10 +3199,10 @@
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C66" ca="1" si="0">INT(RAND()*(99999999-10000000+1)+10000000)</f>
-        <v>92437592</v>
+        <v>24734662</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3">
         <v>3</v>
@@ -3230,10 +3230,10 @@
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>57875676</v>
+        <v>43316177</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -3261,10 +3261,10 @@
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>44312067</v>
+        <v>10797472</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E5">
         <v>3</v>
@@ -3292,10 +3292,10 @@
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>56292984</v>
+        <v>17989816</v>
       </c>
       <c r="D6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E6">
         <v>3</v>
@@ -3323,10 +3323,10 @@
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>10376291</v>
+        <v>84781659</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E7">
         <v>3</v>
@@ -3354,10 +3354,10 @@
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>94502771</v>
+        <v>81517614</v>
       </c>
       <c r="D8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E8">
         <v>3</v>
@@ -3385,10 +3385,10 @@
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="0"/>
-        <v>73455180</v>
+        <v>81720001</v>
       </c>
       <c r="D9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E9">
         <v>3</v>
@@ -3416,10 +3416,10 @@
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="0"/>
-        <v>40073888</v>
+        <v>25857564</v>
       </c>
       <c r="D10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E10">
         <v>3</v>
@@ -3447,10 +3447,10 @@
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="0"/>
-        <v>90499737</v>
+        <v>43243640</v>
       </c>
       <c r="D11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E11">
         <v>3</v>
@@ -3478,10 +3478,10 @@
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="0"/>
-        <v>56787851</v>
+        <v>88438664</v>
       </c>
       <c r="D12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E12">
         <v>3</v>
@@ -3509,10 +3509,10 @@
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="0"/>
-        <v>13601347</v>
+        <v>73662716</v>
       </c>
       <c r="D13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E13">
         <v>3</v>
@@ -3540,10 +3540,10 @@
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="0"/>
-        <v>66367846</v>
+        <v>77303455</v>
       </c>
       <c r="D14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E14">
         <v>3</v>
@@ -3571,10 +3571,10 @@
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="0"/>
-        <v>18492309</v>
+        <v>81150025</v>
       </c>
       <c r="D15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E15">
         <v>3</v>
@@ -3602,10 +3602,10 @@
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="0"/>
-        <v>16136898</v>
+        <v>23463274</v>
       </c>
       <c r="D16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E16">
         <v>3</v>
@@ -3633,10 +3633,10 @@
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="0"/>
-        <v>34827815</v>
+        <v>79285700</v>
       </c>
       <c r="D17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E17">
         <v>3</v>
@@ -3664,10 +3664,10 @@
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="0"/>
-        <v>14965722</v>
+        <v>16297439</v>
       </c>
       <c r="D18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E18">
         <v>3</v>
@@ -3695,10 +3695,10 @@
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="0"/>
-        <v>27412834</v>
+        <v>16582661</v>
       </c>
       <c r="D19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E19">
         <v>3</v>
@@ -3726,10 +3726,10 @@
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="0"/>
-        <v>40906162</v>
+        <v>95117004</v>
       </c>
       <c r="D20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E20">
         <v>3</v>
@@ -3757,10 +3757,10 @@
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="0"/>
-        <v>71260151</v>
+        <v>28033278</v>
       </c>
       <c r="D21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E21">
         <v>3</v>
@@ -3788,10 +3788,10 @@
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="0"/>
-        <v>88780314</v>
+        <v>96776810</v>
       </c>
       <c r="D22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E22">
         <v>3</v>
@@ -3821,10 +3821,10 @@
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="0"/>
-        <v>42755671</v>
+        <v>94527949</v>
       </c>
       <c r="D23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E23">
         <v>3</v>
@@ -3854,10 +3854,10 @@
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="0"/>
-        <v>66957121</v>
+        <v>48803903</v>
       </c>
       <c r="D24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E24">
         <v>3</v>
@@ -3887,10 +3887,10 @@
       </c>
       <c r="C25">
         <f t="shared" ca="1" si="0"/>
-        <v>93081719</v>
+        <v>95041686</v>
       </c>
       <c r="D25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E25">
         <v>3</v>
@@ -3920,10 +3920,10 @@
       </c>
       <c r="C26">
         <f t="shared" ca="1" si="0"/>
-        <v>25352912</v>
+        <v>95979148</v>
       </c>
       <c r="D26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E26">
         <v>3</v>
@@ -3953,10 +3953,10 @@
       </c>
       <c r="C27">
         <f t="shared" ca="1" si="0"/>
-        <v>73978853</v>
+        <v>47717103</v>
       </c>
       <c r="D27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E27">
         <v>3</v>
@@ -3986,10 +3986,10 @@
       </c>
       <c r="C28">
         <f t="shared" ca="1" si="0"/>
-        <v>35774919</v>
+        <v>74255881</v>
       </c>
       <c r="D28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E28">
         <v>3</v>
@@ -4019,10 +4019,10 @@
       </c>
       <c r="C29">
         <f t="shared" ca="1" si="0"/>
-        <v>34709869</v>
+        <v>43514571</v>
       </c>
       <c r="D29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E29">
         <v>3</v>
@@ -4052,10 +4052,10 @@
       </c>
       <c r="C30">
         <f t="shared" ca="1" si="0"/>
-        <v>97245277</v>
+        <v>14764342</v>
       </c>
       <c r="D30">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E30">
         <v>3</v>
@@ -4085,10 +4085,10 @@
       </c>
       <c r="C31">
         <f t="shared" ca="1" si="0"/>
-        <v>38233087</v>
+        <v>80861646</v>
       </c>
       <c r="D31">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E31">
         <v>3</v>
@@ -4118,10 +4118,10 @@
       </c>
       <c r="C32">
         <f t="shared" ca="1" si="0"/>
-        <v>39731563</v>
+        <v>61746359</v>
       </c>
       <c r="D32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E32">
         <v>3</v>
@@ -4151,10 +4151,10 @@
       </c>
       <c r="C33">
         <f t="shared" ca="1" si="0"/>
-        <v>26468543</v>
+        <v>71680436</v>
       </c>
       <c r="D33">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E33">
         <v>3</v>
@@ -4184,10 +4184,10 @@
       </c>
       <c r="C34">
         <f t="shared" ca="1" si="0"/>
-        <v>85057187</v>
+        <v>31501251</v>
       </c>
       <c r="D34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E34">
         <v>3</v>
@@ -4217,10 +4217,10 @@
       </c>
       <c r="C35">
         <f t="shared" ca="1" si="0"/>
-        <v>25486994</v>
+        <v>70487562</v>
       </c>
       <c r="D35">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E35">
         <v>3</v>
@@ -4250,10 +4250,10 @@
       </c>
       <c r="C36">
         <f t="shared" ca="1" si="0"/>
-        <v>52416702</v>
+        <v>57297953</v>
       </c>
       <c r="D36">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E36">
         <v>3</v>
@@ -4283,10 +4283,10 @@
       </c>
       <c r="C37">
         <f t="shared" ca="1" si="0"/>
-        <v>73165930</v>
+        <v>19258404</v>
       </c>
       <c r="D37">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E37">
         <v>3</v>
@@ -4316,10 +4316,10 @@
       </c>
       <c r="C38">
         <f t="shared" ca="1" si="0"/>
-        <v>63024576</v>
+        <v>39769815</v>
       </c>
       <c r="D38">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E38">
         <v>3</v>
@@ -4349,10 +4349,10 @@
       </c>
       <c r="C39">
         <f t="shared" ca="1" si="0"/>
-        <v>73302876</v>
+        <v>83759594</v>
       </c>
       <c r="D39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E39">
         <v>3</v>
@@ -4382,10 +4382,10 @@
       </c>
       <c r="C40">
         <f t="shared" ca="1" si="0"/>
-        <v>11605614</v>
+        <v>96584178</v>
       </c>
       <c r="D40">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E40">
         <v>3</v>
@@ -4415,10 +4415,10 @@
       </c>
       <c r="C41">
         <f t="shared" ca="1" si="0"/>
-        <v>45968858</v>
+        <v>19534948</v>
       </c>
       <c r="D41">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E41">
         <v>3</v>
@@ -4448,10 +4448,10 @@
       </c>
       <c r="C42">
         <f t="shared" ca="1" si="0"/>
-        <v>62791219</v>
+        <v>74221984</v>
       </c>
       <c r="D42">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E42">
         <v>3</v>
@@ -4478,10 +4478,10 @@
       </c>
       <c r="C43">
         <f t="shared" ca="1" si="0"/>
-        <v>47017218</v>
+        <v>43191560</v>
       </c>
       <c r="D43">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E43">
         <v>3</v>
@@ -4508,10 +4508,10 @@
       </c>
       <c r="C44">
         <f t="shared" ca="1" si="0"/>
-        <v>44289756</v>
+        <v>52956556</v>
       </c>
       <c r="D44">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E44">
         <v>3</v>
@@ -4538,10 +4538,10 @@
       </c>
       <c r="C45">
         <f t="shared" ca="1" si="0"/>
-        <v>33269041</v>
+        <v>77582318</v>
       </c>
       <c r="D45">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E45">
         <v>3</v>
@@ -4568,10 +4568,10 @@
       </c>
       <c r="C46">
         <f t="shared" ca="1" si="0"/>
-        <v>64813807</v>
+        <v>35616577</v>
       </c>
       <c r="D46">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E46">
         <v>3</v>
@@ -4598,10 +4598,10 @@
       </c>
       <c r="C47">
         <f t="shared" ca="1" si="0"/>
-        <v>98247431</v>
+        <v>15424112</v>
       </c>
       <c r="D47">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E47">
         <v>3</v>
@@ -4628,10 +4628,10 @@
       </c>
       <c r="C48">
         <f t="shared" ca="1" si="0"/>
-        <v>99711943</v>
+        <v>65998196</v>
       </c>
       <c r="D48">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E48">
         <v>3</v>
@@ -4658,10 +4658,10 @@
       </c>
       <c r="C49">
         <f t="shared" ca="1" si="0"/>
-        <v>38570911</v>
+        <v>20956138</v>
       </c>
       <c r="D49">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E49">
         <v>3</v>
@@ -4688,10 +4688,10 @@
       </c>
       <c r="C50">
         <f t="shared" ca="1" si="0"/>
-        <v>96945542</v>
+        <v>28547798</v>
       </c>
       <c r="D50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E50">
         <v>3</v>
@@ -4718,10 +4718,10 @@
       </c>
       <c r="C51">
         <f t="shared" ca="1" si="0"/>
-        <v>14896824</v>
+        <v>45411426</v>
       </c>
       <c r="D51">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E51">
         <v>3</v>
@@ -4748,10 +4748,10 @@
       </c>
       <c r="C52">
         <f t="shared" ca="1" si="0"/>
-        <v>58319689</v>
+        <v>63662876</v>
       </c>
       <c r="D52">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E52">
         <v>3</v>
@@ -4778,10 +4778,10 @@
       </c>
       <c r="C53">
         <f t="shared" ca="1" si="0"/>
-        <v>39200045</v>
+        <v>79849637</v>
       </c>
       <c r="D53">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E53">
         <v>3</v>
@@ -4808,10 +4808,10 @@
       </c>
       <c r="C54">
         <f t="shared" ca="1" si="0"/>
-        <v>32358895</v>
+        <v>62682687</v>
       </c>
       <c r="D54">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E54">
         <v>3</v>
@@ -4838,10 +4838,10 @@
       </c>
       <c r="C55">
         <f t="shared" ca="1" si="0"/>
-        <v>87984837</v>
+        <v>72872875</v>
       </c>
       <c r="D55">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E55">
         <v>3</v>
@@ -4868,10 +4868,10 @@
       </c>
       <c r="C56">
         <f t="shared" ca="1" si="0"/>
-        <v>15366745</v>
+        <v>14964850</v>
       </c>
       <c r="D56">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E56">
         <v>3</v>
@@ -4898,10 +4898,10 @@
       </c>
       <c r="C57">
         <f t="shared" ca="1" si="0"/>
-        <v>33924367</v>
+        <v>94179389</v>
       </c>
       <c r="D57">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E57">
         <v>3</v>
@@ -4928,10 +4928,10 @@
       </c>
       <c r="C58">
         <f t="shared" ca="1" si="0"/>
-        <v>67197136</v>
+        <v>79732844</v>
       </c>
       <c r="D58">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E58">
         <v>3</v>
@@ -4958,10 +4958,10 @@
       </c>
       <c r="C59">
         <f t="shared" ca="1" si="0"/>
-        <v>48482148</v>
+        <v>83299892</v>
       </c>
       <c r="D59">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E59">
         <v>3</v>
@@ -4988,10 +4988,10 @@
       </c>
       <c r="C60">
         <f t="shared" ca="1" si="0"/>
-        <v>70117259</v>
+        <v>83477161</v>
       </c>
       <c r="D60">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E60">
         <v>3</v>
@@ -5018,10 +5018,10 @@
       </c>
       <c r="C61">
         <f t="shared" ca="1" si="0"/>
-        <v>71349452</v>
+        <v>53017394</v>
       </c>
       <c r="D61">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E61">
         <v>3</v>
@@ -5048,10 +5048,10 @@
       </c>
       <c r="C62">
         <f t="shared" ca="1" si="0"/>
-        <v>30612761</v>
+        <v>75108445</v>
       </c>
       <c r="D62">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E62">
         <v>3</v>
@@ -5078,10 +5078,10 @@
       </c>
       <c r="C63">
         <f t="shared" ca="1" si="0"/>
-        <v>38433196</v>
+        <v>78000366</v>
       </c>
       <c r="D63">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E63">
         <v>3</v>
@@ -5108,10 +5108,10 @@
       </c>
       <c r="C64">
         <f t="shared" ca="1" si="0"/>
-        <v>28407192</v>
+        <v>10057095</v>
       </c>
       <c r="D64">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E64">
         <v>3</v>
@@ -5138,10 +5138,10 @@
       </c>
       <c r="C65">
         <f t="shared" ca="1" si="0"/>
-        <v>60077093</v>
+        <v>96083978</v>
       </c>
       <c r="D65">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E65">
         <v>3</v>
@@ -5168,10 +5168,10 @@
       </c>
       <c r="C66">
         <f t="shared" ca="1" si="0"/>
-        <v>65902094</v>
+        <v>15984479</v>
       </c>
       <c r="D66">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E66">
         <v>3</v>
@@ -5198,10 +5198,10 @@
       </c>
       <c r="C67">
         <f t="shared" ref="C67:C128" ca="1" si="1">INT(RAND()*(99999999-10000000+1)+10000000)</f>
-        <v>70187371</v>
+        <v>13175930</v>
       </c>
       <c r="D67">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E67">
         <v>3</v>
@@ -5228,10 +5228,10 @@
       </c>
       <c r="C68">
         <f t="shared" ca="1" si="1"/>
-        <v>21934541</v>
+        <v>54749831</v>
       </c>
       <c r="D68">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E68">
         <v>3</v>
@@ -5258,10 +5258,10 @@
       </c>
       <c r="C69">
         <f t="shared" ca="1" si="1"/>
-        <v>46479230</v>
+        <v>63507865</v>
       </c>
       <c r="D69">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E69">
         <v>3</v>
@@ -5288,10 +5288,10 @@
       </c>
       <c r="C70">
         <f t="shared" ca="1" si="1"/>
-        <v>59486175</v>
+        <v>14663483</v>
       </c>
       <c r="D70">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E70">
         <v>3</v>
@@ -5318,10 +5318,10 @@
       </c>
       <c r="C71">
         <f t="shared" ca="1" si="1"/>
-        <v>10358373</v>
+        <v>26306703</v>
       </c>
       <c r="D71">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E71">
         <v>3</v>
@@ -5348,10 +5348,10 @@
       </c>
       <c r="C72">
         <f t="shared" ca="1" si="1"/>
-        <v>98698687</v>
+        <v>72387038</v>
       </c>
       <c r="D72">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E72">
         <v>3</v>
@@ -5378,10 +5378,10 @@
       </c>
       <c r="C73">
         <f t="shared" ca="1" si="1"/>
-        <v>81915927</v>
+        <v>61580251</v>
       </c>
       <c r="D73">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E73">
         <v>3</v>
@@ -5408,10 +5408,10 @@
       </c>
       <c r="C74">
         <f t="shared" ca="1" si="1"/>
-        <v>85132127</v>
+        <v>79690099</v>
       </c>
       <c r="D74">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E74">
         <v>3</v>
@@ -5438,10 +5438,10 @@
       </c>
       <c r="C75">
         <f t="shared" ca="1" si="1"/>
-        <v>12826463</v>
+        <v>67069698</v>
       </c>
       <c r="D75">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E75">
         <v>3</v>
@@ -5468,10 +5468,10 @@
       </c>
       <c r="C76">
         <f t="shared" ca="1" si="1"/>
-        <v>62162703</v>
+        <v>25917898</v>
       </c>
       <c r="D76">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E76">
         <v>3</v>
@@ -5498,10 +5498,10 @@
       </c>
       <c r="C77">
         <f t="shared" ca="1" si="1"/>
-        <v>36662127</v>
+        <v>48572722</v>
       </c>
       <c r="D77">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E77">
         <v>3</v>
@@ -5528,10 +5528,10 @@
       </c>
       <c r="C78">
         <f t="shared" ca="1" si="1"/>
-        <v>53444054</v>
+        <v>83155057</v>
       </c>
       <c r="D78">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E78">
         <v>3</v>
@@ -5558,10 +5558,10 @@
       </c>
       <c r="C79">
         <f t="shared" ca="1" si="1"/>
-        <v>75737837</v>
+        <v>35740498</v>
       </c>
       <c r="D79">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E79">
         <v>3</v>
@@ -5588,10 +5588,10 @@
       </c>
       <c r="C80">
         <f t="shared" ca="1" si="1"/>
-        <v>21292829</v>
+        <v>15469849</v>
       </c>
       <c r="D80">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E80">
         <v>3</v>
@@ -5618,10 +5618,10 @@
       </c>
       <c r="C81">
         <f t="shared" ca="1" si="1"/>
-        <v>73476924</v>
+        <v>63258753</v>
       </c>
       <c r="D81">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E81">
         <v>3</v>
@@ -5648,10 +5648,10 @@
       </c>
       <c r="C82">
         <f t="shared" ca="1" si="1"/>
-        <v>20372024</v>
+        <v>38375997</v>
       </c>
       <c r="D82">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E82">
         <v>3</v>
@@ -5678,10 +5678,10 @@
       </c>
       <c r="C83">
         <f t="shared" ca="1" si="1"/>
-        <v>49994205</v>
+        <v>23863810</v>
       </c>
       <c r="D83">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E83">
         <v>3</v>
@@ -5708,10 +5708,10 @@
       </c>
       <c r="C84">
         <f t="shared" ca="1" si="1"/>
-        <v>19261730</v>
+        <v>15334102</v>
       </c>
       <c r="D84">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E84">
         <v>3</v>
@@ -5738,10 +5738,10 @@
       </c>
       <c r="C85">
         <f t="shared" ca="1" si="1"/>
-        <v>10317607</v>
+        <v>43378809</v>
       </c>
       <c r="D85">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E85">
         <v>3</v>
@@ -5768,10 +5768,10 @@
       </c>
       <c r="C86">
         <f t="shared" ca="1" si="1"/>
-        <v>10549344</v>
+        <v>69041365</v>
       </c>
       <c r="D86">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E86">
         <v>3</v>
@@ -5798,10 +5798,10 @@
       </c>
       <c r="C87">
         <f t="shared" ca="1" si="1"/>
-        <v>29683449</v>
+        <v>54930727</v>
       </c>
       <c r="D87">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E87">
         <v>3</v>
@@ -5828,10 +5828,10 @@
       </c>
       <c r="C88">
         <f t="shared" ca="1" si="1"/>
-        <v>19578708</v>
+        <v>23347982</v>
       </c>
       <c r="D88">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E88">
         <v>3</v>
@@ -5858,10 +5858,10 @@
       </c>
       <c r="C89">
         <f t="shared" ca="1" si="1"/>
-        <v>52493990</v>
+        <v>90297619</v>
       </c>
       <c r="D89">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E89">
         <v>3</v>
@@ -5888,10 +5888,10 @@
       </c>
       <c r="C90">
         <f t="shared" ca="1" si="1"/>
-        <v>13531247</v>
+        <v>12406115</v>
       </c>
       <c r="D90">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E90">
         <v>3</v>
@@ -5918,10 +5918,10 @@
       </c>
       <c r="C91">
         <f t="shared" ca="1" si="1"/>
-        <v>53428219</v>
+        <v>17037108</v>
       </c>
       <c r="D91">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E91">
         <v>3</v>
@@ -5948,10 +5948,10 @@
       </c>
       <c r="C92">
         <f t="shared" ca="1" si="1"/>
-        <v>49517737</v>
+        <v>36465482</v>
       </c>
       <c r="D92">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E92">
         <v>3</v>
@@ -5978,10 +5978,10 @@
       </c>
       <c r="C93">
         <f t="shared" ca="1" si="1"/>
-        <v>73331768</v>
+        <v>45613576</v>
       </c>
       <c r="D93">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E93">
         <v>3</v>
@@ -6008,10 +6008,10 @@
       </c>
       <c r="C94">
         <f t="shared" ca="1" si="1"/>
-        <v>17677471</v>
+        <v>13192514</v>
       </c>
       <c r="D94">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E94">
         <v>3</v>
@@ -6038,10 +6038,10 @@
       </c>
       <c r="C95">
         <f t="shared" ca="1" si="1"/>
-        <v>70591266</v>
+        <v>84791911</v>
       </c>
       <c r="D95">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E95">
         <v>3</v>
@@ -6068,10 +6068,10 @@
       </c>
       <c r="C96">
         <f t="shared" ca="1" si="1"/>
-        <v>75562442</v>
+        <v>72367373</v>
       </c>
       <c r="D96">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E96">
         <v>3</v>
@@ -6098,10 +6098,10 @@
       </c>
       <c r="C97">
         <f t="shared" ca="1" si="1"/>
-        <v>25147775</v>
+        <v>73277018</v>
       </c>
       <c r="D97">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E97">
         <v>3</v>
@@ -6128,10 +6128,10 @@
       </c>
       <c r="C98">
         <f t="shared" ca="1" si="1"/>
-        <v>66733233</v>
+        <v>84050182</v>
       </c>
       <c r="D98">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E98">
         <v>3</v>
@@ -6158,10 +6158,10 @@
       </c>
       <c r="C99">
         <f t="shared" ca="1" si="1"/>
-        <v>92958195</v>
+        <v>42497239</v>
       </c>
       <c r="D99">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E99">
         <v>3</v>
@@ -6188,10 +6188,10 @@
       </c>
       <c r="C100">
         <f t="shared" ca="1" si="1"/>
-        <v>36844352</v>
+        <v>41647234</v>
       </c>
       <c r="D100">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E100">
         <v>3</v>
@@ -6218,10 +6218,10 @@
       </c>
       <c r="C101">
         <f t="shared" ca="1" si="1"/>
-        <v>80150955</v>
+        <v>36702702</v>
       </c>
       <c r="D101">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E101">
         <v>3</v>
@@ -6248,10 +6248,10 @@
       </c>
       <c r="C102">
         <f t="shared" ca="1" si="1"/>
-        <v>44468692</v>
+        <v>63638833</v>
       </c>
       <c r="D102">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E102">
         <v>3</v>
@@ -6278,10 +6278,10 @@
       </c>
       <c r="C103">
         <f t="shared" ca="1" si="1"/>
-        <v>29164759</v>
+        <v>67205886</v>
       </c>
       <c r="D103">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E103">
         <v>3</v>
@@ -6308,10 +6308,10 @@
       </c>
       <c r="C104">
         <f t="shared" ca="1" si="1"/>
-        <v>21538793</v>
+        <v>28033239</v>
       </c>
       <c r="D104">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E104">
         <v>3</v>
@@ -6338,10 +6338,10 @@
       </c>
       <c r="C105">
         <f t="shared" ca="1" si="1"/>
-        <v>57693357</v>
+        <v>71442506</v>
       </c>
       <c r="D105">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E105">
         <v>3</v>
@@ -6368,10 +6368,10 @@
       </c>
       <c r="C106">
         <f t="shared" ca="1" si="1"/>
-        <v>74771594</v>
+        <v>20481602</v>
       </c>
       <c r="D106">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E106">
         <v>3</v>
@@ -6398,10 +6398,10 @@
       </c>
       <c r="C107">
         <f t="shared" ca="1" si="1"/>
-        <v>39558174</v>
+        <v>68045099</v>
       </c>
       <c r="D107">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E107">
         <v>3</v>
@@ -6428,10 +6428,10 @@
       </c>
       <c r="C108">
         <f t="shared" ca="1" si="1"/>
-        <v>22538555</v>
+        <v>26849310</v>
       </c>
       <c r="D108">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E108">
         <v>3</v>
@@ -6458,10 +6458,10 @@
       </c>
       <c r="C109">
         <f t="shared" ca="1" si="1"/>
-        <v>85777649</v>
+        <v>62530626</v>
       </c>
       <c r="D109">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E109">
         <v>3</v>
@@ -6488,10 +6488,10 @@
       </c>
       <c r="C110">
         <f t="shared" ca="1" si="1"/>
-        <v>96573665</v>
+        <v>66661105</v>
       </c>
       <c r="D110">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E110">
         <v>3</v>
@@ -6518,10 +6518,10 @@
       </c>
       <c r="C111">
         <f t="shared" ca="1" si="1"/>
-        <v>10754106</v>
+        <v>49932268</v>
       </c>
       <c r="D111">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E111">
         <v>3</v>
@@ -6548,10 +6548,10 @@
       </c>
       <c r="C112">
         <f t="shared" ca="1" si="1"/>
-        <v>19644228</v>
+        <v>95379609</v>
       </c>
       <c r="D112">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E112">
         <v>3</v>
@@ -6578,10 +6578,10 @@
       </c>
       <c r="C113">
         <f t="shared" ca="1" si="1"/>
-        <v>54835429</v>
+        <v>57687959</v>
       </c>
       <c r="D113">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E113">
         <v>3</v>
@@ -6608,10 +6608,10 @@
       </c>
       <c r="C114">
         <f t="shared" ca="1" si="1"/>
-        <v>34226848</v>
+        <v>94909250</v>
       </c>
       <c r="D114">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E114">
         <v>3</v>
@@ -6638,10 +6638,10 @@
       </c>
       <c r="C115">
         <f t="shared" ca="1" si="1"/>
-        <v>64898360</v>
+        <v>62053210</v>
       </c>
       <c r="D115">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E115">
         <v>3</v>
@@ -6668,10 +6668,10 @@
       </c>
       <c r="C116">
         <f t="shared" ca="1" si="1"/>
-        <v>27743612</v>
+        <v>43282694</v>
       </c>
       <c r="D116">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E116">
         <v>3</v>
@@ -6698,10 +6698,10 @@
       </c>
       <c r="C117">
         <f t="shared" ca="1" si="1"/>
-        <v>28010396</v>
+        <v>32638362</v>
       </c>
       <c r="D117">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E117">
         <v>3</v>
@@ -6728,10 +6728,10 @@
       </c>
       <c r="C118">
         <f t="shared" ca="1" si="1"/>
-        <v>80955449</v>
+        <v>97207038</v>
       </c>
       <c r="D118">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E118">
         <v>3</v>
@@ -6758,10 +6758,10 @@
       </c>
       <c r="C119">
         <f t="shared" ca="1" si="1"/>
-        <v>75013466</v>
+        <v>46285562</v>
       </c>
       <c r="D119">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E119">
         <v>3</v>
@@ -6788,10 +6788,10 @@
       </c>
       <c r="C120">
         <f t="shared" ca="1" si="1"/>
-        <v>68822283</v>
+        <v>24737512</v>
       </c>
       <c r="D120">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E120">
         <v>3</v>
@@ -6818,10 +6818,10 @@
       </c>
       <c r="C121">
         <f t="shared" ca="1" si="1"/>
-        <v>19659266</v>
+        <v>91461830</v>
       </c>
       <c r="D121">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E121">
         <v>3</v>
@@ -6848,10 +6848,10 @@
       </c>
       <c r="C122">
         <f t="shared" ca="1" si="1"/>
-        <v>31036463</v>
+        <v>26869334</v>
       </c>
       <c r="D122">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E122">
         <v>3</v>
@@ -6878,10 +6878,10 @@
       </c>
       <c r="C123">
         <f t="shared" ca="1" si="1"/>
-        <v>19452666</v>
+        <v>14194875</v>
       </c>
       <c r="D123">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E123">
         <v>3</v>
@@ -6908,10 +6908,10 @@
       </c>
       <c r="C124">
         <f t="shared" ca="1" si="1"/>
-        <v>18114875</v>
+        <v>55608011</v>
       </c>
       <c r="D124">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E124">
         <v>3</v>
@@ -6938,10 +6938,10 @@
       </c>
       <c r="C125">
         <f t="shared" ca="1" si="1"/>
-        <v>43084971</v>
+        <v>74382496</v>
       </c>
       <c r="D125">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E125">
         <v>3</v>
@@ -6968,10 +6968,10 @@
       </c>
       <c r="C126">
         <f t="shared" ca="1" si="1"/>
-        <v>81973415</v>
+        <v>95597330</v>
       </c>
       <c r="D126">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E126">
         <v>3</v>
@@ -6998,10 +6998,10 @@
       </c>
       <c r="C127">
         <f t="shared" ca="1" si="1"/>
-        <v>15961632</v>
+        <v>53641291</v>
       </c>
       <c r="D127">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E127">
         <v>3</v>
@@ -7028,10 +7028,10 @@
       </c>
       <c r="C128">
         <f t="shared" ca="1" si="1"/>
-        <v>95561238</v>
+        <v>17629176</v>
       </c>
       <c r="D128">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E128">
         <v>3</v>
@@ -7058,10 +7058,10 @@
       </c>
       <c r="C129">
         <f t="shared" ref="C129:C176" ca="1" si="2">INT(RAND()*(99999999-10000000+1)+10000000)</f>
-        <v>95688497</v>
+        <v>36080278</v>
       </c>
       <c r="D129">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E129">
         <v>3</v>
@@ -7088,10 +7088,10 @@
       </c>
       <c r="C130">
         <f t="shared" ca="1" si="2"/>
-        <v>13850384</v>
+        <v>74522465</v>
       </c>
       <c r="D130">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E130">
         <v>3</v>
@@ -7118,10 +7118,10 @@
       </c>
       <c r="C131">
         <f t="shared" ca="1" si="2"/>
-        <v>79224942</v>
+        <v>66057344</v>
       </c>
       <c r="D131">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E131">
         <v>3</v>
@@ -7148,10 +7148,10 @@
       </c>
       <c r="C132">
         <f t="shared" ca="1" si="2"/>
-        <v>42256350</v>
+        <v>57985730</v>
       </c>
       <c r="D132">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E132">
         <v>3</v>
@@ -7178,10 +7178,10 @@
       </c>
       <c r="C133">
         <f t="shared" ca="1" si="2"/>
-        <v>49766441</v>
+        <v>94655940</v>
       </c>
       <c r="D133">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E133">
         <v>3</v>
@@ -7208,10 +7208,10 @@
       </c>
       <c r="C134">
         <f t="shared" ca="1" si="2"/>
-        <v>95590725</v>
+        <v>30934153</v>
       </c>
       <c r="D134">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E134">
         <v>3</v>
@@ -7238,10 +7238,10 @@
       </c>
       <c r="C135">
         <f t="shared" ca="1" si="2"/>
-        <v>49106317</v>
+        <v>43418214</v>
       </c>
       <c r="D135">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E135">
         <v>3</v>
@@ -7268,10 +7268,10 @@
       </c>
       <c r="C136">
         <f t="shared" ca="1" si="2"/>
-        <v>55405195</v>
+        <v>16749791</v>
       </c>
       <c r="D136">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E136">
         <v>3</v>
@@ -7298,10 +7298,10 @@
       </c>
       <c r="C137">
         <f t="shared" ca="1" si="2"/>
-        <v>79135996</v>
+        <v>18040465</v>
       </c>
       <c r="D137">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E137">
         <v>3</v>
@@ -7328,10 +7328,10 @@
       </c>
       <c r="C138">
         <f t="shared" ca="1" si="2"/>
-        <v>76655985</v>
+        <v>56835333</v>
       </c>
       <c r="D138">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E138">
         <v>3</v>
@@ -7358,10 +7358,10 @@
       </c>
       <c r="C139">
         <f t="shared" ca="1" si="2"/>
-        <v>51830082</v>
+        <v>82895330</v>
       </c>
       <c r="D139">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E139">
         <v>3</v>
@@ -7388,10 +7388,10 @@
       </c>
       <c r="C140">
         <f t="shared" ca="1" si="2"/>
-        <v>68856921</v>
+        <v>20451810</v>
       </c>
       <c r="D140">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E140">
         <v>3</v>
@@ -7418,10 +7418,10 @@
       </c>
       <c r="C141">
         <f t="shared" ca="1" si="2"/>
-        <v>95454039</v>
+        <v>37549361</v>
       </c>
       <c r="D141">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E141">
         <v>3</v>
@@ -7448,10 +7448,10 @@
       </c>
       <c r="C142">
         <f t="shared" ca="1" si="2"/>
-        <v>65866055</v>
+        <v>38872551</v>
       </c>
       <c r="D142">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E142">
         <v>3</v>
@@ -7478,10 +7478,10 @@
       </c>
       <c r="C143">
         <f t="shared" ca="1" si="2"/>
-        <v>89071286</v>
+        <v>22107039</v>
       </c>
       <c r="D143">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E143">
         <v>3</v>
@@ -7508,10 +7508,10 @@
       </c>
       <c r="C144">
         <f t="shared" ca="1" si="2"/>
-        <v>68137032</v>
+        <v>72412640</v>
       </c>
       <c r="D144">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E144">
         <v>3</v>
@@ -7538,10 +7538,10 @@
       </c>
       <c r="C145">
         <f t="shared" ca="1" si="2"/>
-        <v>81471361</v>
+        <v>11414203</v>
       </c>
       <c r="D145">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E145">
         <v>3</v>
@@ -7568,10 +7568,10 @@
       </c>
       <c r="C146">
         <f t="shared" ca="1" si="2"/>
-        <v>69524469</v>
+        <v>30072024</v>
       </c>
       <c r="D146">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E146">
         <v>3</v>
@@ -7598,10 +7598,10 @@
       </c>
       <c r="C147">
         <f t="shared" ca="1" si="2"/>
-        <v>91234077</v>
+        <v>88754197</v>
       </c>
       <c r="D147">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E147">
         <v>3</v>
@@ -7628,10 +7628,10 @@
       </c>
       <c r="C148">
         <f t="shared" ca="1" si="2"/>
-        <v>16467130</v>
+        <v>87521294</v>
       </c>
       <c r="D148">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E148">
         <v>3</v>
@@ -7658,10 +7658,10 @@
       </c>
       <c r="C149">
         <f t="shared" ca="1" si="2"/>
-        <v>24289494</v>
+        <v>60068637</v>
       </c>
       <c r="D149">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E149">
         <v>3</v>
@@ -7688,10 +7688,10 @@
       </c>
       <c r="C150">
         <f t="shared" ca="1" si="2"/>
-        <v>41639732</v>
+        <v>98845400</v>
       </c>
       <c r="D150">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E150">
         <v>3</v>
@@ -7718,10 +7718,10 @@
       </c>
       <c r="C151">
         <f t="shared" ca="1" si="2"/>
-        <v>94301955</v>
+        <v>47415761</v>
       </c>
       <c r="D151">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E151">
         <v>3</v>
@@ -7748,10 +7748,10 @@
       </c>
       <c r="C152">
         <f t="shared" ca="1" si="2"/>
-        <v>19863041</v>
+        <v>53653957</v>
       </c>
       <c r="D152">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E152">
         <v>3</v>
@@ -7778,10 +7778,10 @@
       </c>
       <c r="C153">
         <f t="shared" ca="1" si="2"/>
-        <v>31926733</v>
+        <v>15903602</v>
       </c>
       <c r="D153">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E153">
         <v>3</v>
@@ -7808,10 +7808,10 @@
       </c>
       <c r="C154">
         <f t="shared" ca="1" si="2"/>
-        <v>60295297</v>
+        <v>15146555</v>
       </c>
       <c r="D154">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E154">
         <v>3</v>
@@ -7838,10 +7838,10 @@
       </c>
       <c r="C155">
         <f t="shared" ca="1" si="2"/>
-        <v>23382409</v>
+        <v>43915880</v>
       </c>
       <c r="D155">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E155">
         <v>3</v>
@@ -7868,10 +7868,10 @@
       </c>
       <c r="C156">
         <f t="shared" ca="1" si="2"/>
-        <v>43312171</v>
+        <v>75135197</v>
       </c>
       <c r="D156">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E156">
         <v>3</v>
@@ -7898,10 +7898,10 @@
       </c>
       <c r="C157">
         <f t="shared" ca="1" si="2"/>
-        <v>78982883</v>
+        <v>91739764</v>
       </c>
       <c r="D157">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E157">
         <v>3</v>
@@ -7928,10 +7928,10 @@
       </c>
       <c r="C158">
         <f t="shared" ca="1" si="2"/>
-        <v>86216221</v>
+        <v>82370322</v>
       </c>
       <c r="D158">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E158">
         <v>3</v>
@@ -7958,10 +7958,10 @@
       </c>
       <c r="C159">
         <f t="shared" ca="1" si="2"/>
-        <v>84226250</v>
+        <v>95332779</v>
       </c>
       <c r="D159">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E159">
         <v>3</v>
@@ -7988,10 +7988,10 @@
       </c>
       <c r="C160">
         <f t="shared" ca="1" si="2"/>
-        <v>35121814</v>
+        <v>18519133</v>
       </c>
       <c r="D160">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E160">
         <v>3</v>
@@ -8018,10 +8018,10 @@
       </c>
       <c r="C161">
         <f t="shared" ca="1" si="2"/>
-        <v>20029911</v>
+        <v>76257975</v>
       </c>
       <c r="D161">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E161">
         <v>3</v>
@@ -8048,10 +8048,10 @@
       </c>
       <c r="C162">
         <f t="shared" ca="1" si="2"/>
-        <v>86014471</v>
+        <v>34980038</v>
       </c>
       <c r="D162">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E162">
         <v>3</v>
@@ -8078,10 +8078,10 @@
       </c>
       <c r="C163">
         <f t="shared" ca="1" si="2"/>
-        <v>18530286</v>
+        <v>37952980</v>
       </c>
       <c r="D163">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E163">
         <v>3</v>
@@ -8108,10 +8108,10 @@
       </c>
       <c r="C164">
         <f t="shared" ca="1" si="2"/>
-        <v>82676750</v>
+        <v>94083117</v>
       </c>
       <c r="D164">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E164">
         <v>3</v>
@@ -8138,10 +8138,10 @@
       </c>
       <c r="C165">
         <f t="shared" ca="1" si="2"/>
-        <v>60661387</v>
+        <v>25766571</v>
       </c>
       <c r="D165">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E165">
         <v>3</v>
@@ -8168,10 +8168,10 @@
       </c>
       <c r="C166">
         <f t="shared" ca="1" si="2"/>
-        <v>68227167</v>
+        <v>17656000</v>
       </c>
       <c r="D166">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E166">
         <v>3</v>
@@ -8198,10 +8198,10 @@
       </c>
       <c r="C167">
         <f t="shared" ca="1" si="2"/>
-        <v>22319035</v>
+        <v>98831920</v>
       </c>
       <c r="D167">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E167">
         <v>3</v>
@@ -8228,10 +8228,10 @@
       </c>
       <c r="C168">
         <f t="shared" ca="1" si="2"/>
-        <v>56710818</v>
+        <v>34548641</v>
       </c>
       <c r="D168">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E168">
         <v>3</v>
@@ -8258,10 +8258,10 @@
       </c>
       <c r="C169">
         <f t="shared" ca="1" si="2"/>
-        <v>21853517</v>
+        <v>53402294</v>
       </c>
       <c r="D169">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E169">
         <v>3</v>
@@ -8288,10 +8288,10 @@
       </c>
       <c r="C170">
         <f t="shared" ca="1" si="2"/>
-        <v>84598970</v>
+        <v>24701905</v>
       </c>
       <c r="D170">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E170">
         <v>3</v>
@@ -8318,10 +8318,10 @@
       </c>
       <c r="C171">
         <f t="shared" ca="1" si="2"/>
-        <v>67719224</v>
+        <v>49628456</v>
       </c>
       <c r="D171">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E171">
         <v>3</v>
@@ -8348,10 +8348,10 @@
       </c>
       <c r="C172">
         <f t="shared" ca="1" si="2"/>
-        <v>20331072</v>
+        <v>99950137</v>
       </c>
       <c r="D172">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E172">
         <v>3</v>
@@ -8378,10 +8378,10 @@
       </c>
       <c r="C173">
         <f t="shared" ca="1" si="2"/>
-        <v>75525011</v>
+        <v>85801113</v>
       </c>
       <c r="D173">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E173">
         <v>3</v>
@@ -8408,10 +8408,10 @@
       </c>
       <c r="C174">
         <f t="shared" ca="1" si="2"/>
-        <v>84743781</v>
+        <v>64954188</v>
       </c>
       <c r="D174">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E174">
         <v>3</v>
@@ -8438,10 +8438,10 @@
       </c>
       <c r="C175">
         <f t="shared" ca="1" si="2"/>
-        <v>25703669</v>
+        <v>21697260</v>
       </c>
       <c r="D175">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E175">
         <v>3</v>
@@ -8468,10 +8468,10 @@
       </c>
       <c r="C176">
         <f t="shared" ca="1" si="2"/>
-        <v>44884334</v>
+        <v>81956795</v>
       </c>
       <c r="D176">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E176">
         <v>3</v>

</xml_diff>